<commit_message>
Signed-off-by: Mr. Snow <Mr. Snow>
</commit_message>
<xml_diff>
--- a/教程/kad操作一览表.xlsx
+++ b/教程/kad操作一览表.xlsx
@@ -12,8 +12,9 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11370"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="process" sheetId="1" r:id="rId1"/>
+    <sheet name="opcode" sheetId="2" r:id="rId2"/>
+    <sheet name="Tag" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="319">
   <si>
     <t>process</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -123,6 +124,9 @@
     <t>KADEMLIA2_FIREWALLUDP</t>
   </si>
   <si>
+    <t>#define</t>
+  </si>
+  <si>
     <t>KADEMLIA2_PUBLISH_SOURCE_REQ</t>
   </si>
   <si>
@@ -361,6 +365,628 @@
   </si>
   <si>
     <t xml:space="preserve">// &lt;errorcode [1]&gt;&lt;UDPPort_Used [2]&gt;                                                                 </t>
+  </si>
+  <si>
+    <t>#define  FT_FILENAME</t>
+  </si>
+  <si>
+    <t>// &lt;string&gt;</t>
+  </si>
+  <si>
+    <t>#define TAG_FILENAME</t>
+  </si>
+  <si>
+    <t>\x01</t>
+  </si>
+  <si>
+    <t>#define  FT_FILESIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x02</t>
+  </si>
+  <si>
+    <t>// &lt;uint32&gt; (or &lt;uint64&gt; when supported)</t>
+  </si>
+  <si>
+    <t>#define TAG_FILESIZE</t>
+  </si>
+  <si>
+    <t>\x02</t>
+  </si>
+  <si>
+    <t>// &lt;uint32&gt;</t>
+  </si>
+  <si>
+    <t>#define  FT_FILESIZE_HI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x3A</t>
+  </si>
+  <si>
+    <t>#define TAG_FILESIZE_HI</t>
+  </si>
+  <si>
+    <t>\x3A</t>
+  </si>
+  <si>
+    <t>#define  FT_FILETYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x03</t>
+  </si>
+  <si>
+    <t>#define TAG_FILETYPE</t>
+  </si>
+  <si>
+    <t>\x03</t>
+  </si>
+  <si>
+    <t>#define  FT_FILEFORMAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x04</t>
+  </si>
+  <si>
+    <t>#define TAG_FILEFORMAT</t>
+  </si>
+  <si>
+    <t>\x04</t>
+  </si>
+  <si>
+    <t>#define  FT_LASTSEENCOMPLETE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x05</t>
+  </si>
+  <si>
+    <t>#define TAG_COLLECTION</t>
+  </si>
+  <si>
+    <t>\x05</t>
+  </si>
+  <si>
+    <t>TAG_PART_PATH</t>
+  </si>
+  <si>
+    <t>\x06</t>
+  </si>
+  <si>
+    <t>TAG_PART_HASH</t>
+  </si>
+  <si>
+    <t>\x07</t>
+  </si>
+  <si>
+    <t>#define  FT_TRANSFERRED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x08</t>
+  </si>
+  <si>
+    <t>TAG_TRANSFERRED</t>
+  </si>
+  <si>
+    <t>\x08</t>
+  </si>
+  <si>
+    <t>#define  FT_GAPSTART</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x09</t>
+  </si>
+  <si>
+    <t>TAG_GAPSTART</t>
+  </si>
+  <si>
+    <t>\x09</t>
+  </si>
+  <si>
+    <t>#define  FT_GAPEND</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x0A</t>
+  </si>
+  <si>
+    <t>TAG_GAPEND</t>
+  </si>
+  <si>
+    <t>\x0A</t>
+  </si>
+  <si>
+    <t>#define  FT_DESCRIPTION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x0B</t>
+  </si>
+  <si>
+    <t>TAG_DESCRIPTION</t>
+  </si>
+  <si>
+    <t>\x0B</t>
+  </si>
+  <si>
+    <t>TAG_PING</t>
+  </si>
+  <si>
+    <t>\x0C</t>
+  </si>
+  <si>
+    <t>TAG_FAIL</t>
+  </si>
+  <si>
+    <t>\x0D</t>
+  </si>
+  <si>
+    <t>TAG_PREFERENCE</t>
+  </si>
+  <si>
+    <t>\x0E</t>
+  </si>
+  <si>
+    <t>#define TAG_PORT</t>
+  </si>
+  <si>
+    <t>\x0F</t>
+  </si>
+  <si>
+    <t>#define TAG_IP_ADDRESS</t>
+  </si>
+  <si>
+    <t>\x10</t>
+  </si>
+  <si>
+    <t>#define TAG_VERSION</t>
+  </si>
+  <si>
+    <t>\x11</t>
+  </si>
+  <si>
+    <t>#define  FT_PARTFILENAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x12</t>
+  </si>
+  <si>
+    <t>#define TAG_PARTFILENAME</t>
+  </si>
+  <si>
+    <t>\x12</t>
+  </si>
+  <si>
+    <t>//#define FT_PRIORITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x13</t>
+  </si>
+  <si>
+    <t>// Not used anymore</t>
+  </si>
+  <si>
+    <t>#define TAG_PRIORITY</t>
+  </si>
+  <si>
+    <t>\x13</t>
+  </si>
+  <si>
+    <t>#define  FT_STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x14</t>
+  </si>
+  <si>
+    <t>#define TAG_STATUS</t>
+  </si>
+  <si>
+    <t>\x14</t>
+  </si>
+  <si>
+    <t>#define  FT_SOURCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x15</t>
+  </si>
+  <si>
+    <t>#define TAG_SOURCES</t>
+  </si>
+  <si>
+    <t>\x15</t>
+  </si>
+  <si>
+    <t>#define  FT_PERMISSIONS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x16</t>
+  </si>
+  <si>
+    <t>#define TAG_PERMISSIONS</t>
+  </si>
+  <si>
+    <t>\x16</t>
+  </si>
+  <si>
+    <t>//#define FT_ULPRIORITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x17</t>
+  </si>
+  <si>
+    <t>#define TAG_PARTS</t>
+  </si>
+  <si>
+    <t>\x17</t>
+  </si>
+  <si>
+    <t>#define  FT_DLPRIORITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x18</t>
+  </si>
+  <si>
+    <t>// Was 13</t>
+  </si>
+  <si>
+    <t>#define  FT_ULPRIORITY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x19</t>
+  </si>
+  <si>
+    <t>// Was 17</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_COMPRESSION</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x1A</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_CORRUPTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x1B</t>
+  </si>
+  <si>
+    <t>#define  FT_KADLASTPUBLISHKEY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x20</t>
+  </si>
+  <si>
+    <t>#define  FT_KADLASTPUBLISHSRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x21</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_FLAGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x22</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_DL_ACTIVE_TIME</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x23</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_CORRUPTEDPARTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x24</t>
+  </si>
+  <si>
+    <t>#define  FT_DL_PREVIEW</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x25</t>
+  </si>
+  <si>
+    <t>#define  FT_KADLASTPUBLISHNOTES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">// &lt;uint32&gt; </t>
+  </si>
+  <si>
+    <t>#define  FT_AICH_HASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x27</t>
+  </si>
+  <si>
+    <t>#define  FT_FILEHASH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x28</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_COMPLETE_SOURCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x30</t>
+  </si>
+  <si>
+    <t>// nr. of sources which share a complete version of the associated file (supported by eserver 16.46+)</t>
+  </si>
+  <si>
+    <t>#define TAG_COMPLETE_SOURCES</t>
+  </si>
+  <si>
+    <t>\x30</t>
+  </si>
+  <si>
+    <t>#define  FT_COLLECTIONAUTHOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x31</t>
+  </si>
+  <si>
+    <t>#define  FT_COLLECTIONAUTHORKEY  0x32</t>
+  </si>
+  <si>
+    <t>#define  FT_PUBLISHINFO</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x33</t>
+  </si>
+  <si>
+    <t>#define TAG_PUBLISHINFO</t>
+  </si>
+  <si>
+    <t>\x33</t>
+  </si>
+  <si>
+    <t>#define  FT_LASTSHARED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x34</t>
+  </si>
+  <si>
+    <t>#define  FT_AICHHASHSET</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x35</t>
+  </si>
+  <si>
+    <t>TAG_KADAICHHASHPUB</t>
+  </si>
+  <si>
+    <t>\x36</t>
+  </si>
+  <si>
+    <t>// &lt;AICH Hash&gt;</t>
+  </si>
+  <si>
+    <t>#define TAG_KADAICHHASHRESULT</t>
+  </si>
+  <si>
+    <t>\x37</t>
+  </si>
+  <si>
+    <t>// &lt;Count 1&gt;{&lt;Publishers 1&gt;&lt;AICH Hash&gt; Count}</t>
+  </si>
+  <si>
+    <t>// statistic</t>
+  </si>
+  <si>
+    <t>#define  FT_ATTRANSFERRED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x50</t>
+  </si>
+  <si>
+    <t>#define  FT_ATREQUESTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x51</t>
+  </si>
+  <si>
+    <t>#define  FT_ATACCEPTED</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x52</t>
+  </si>
+  <si>
+    <t>#define  FT_CATEGORY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x53</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_ATTRANSFERREDHI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x54</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_MAXSOURCES</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x55</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_MEDIA_ARTIST</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0xD0</t>
+  </si>
+  <si>
+    <t>TAG_MEDIA_ARTIST</t>
+  </si>
+  <si>
+    <t>\xD0</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_MEDIA_ALBUM</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0xD1</t>
+  </si>
+  <si>
+    <t>TAG_MEDIA_ALBUM</t>
+  </si>
+  <si>
+    <t>\xD1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_MEDIA_TITLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0xD2</t>
+  </si>
+  <si>
+    <t>TAG_MEDIA_TITLE</t>
+  </si>
+  <si>
+    <t>\xD2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_MEDIA_LENGTH</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0xD3</t>
+  </si>
+  <si>
+    <t>// &lt;uint32&gt; !!!</t>
+  </si>
+  <si>
+    <t>TAG_MEDIA_LENGTH</t>
+  </si>
+  <si>
+    <t>\xD3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_MEDIA_BITRATE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0xD4</t>
+  </si>
+  <si>
+    <t>TAG_MEDIA_BITRATE</t>
+  </si>
+  <si>
+    <t>\xD4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> FT_MEDIA_CODEC</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0xD5</t>
+  </si>
+  <si>
+    <t>TAG_MEDIA_CODEC</t>
+  </si>
+  <si>
+    <t>\xD5</t>
+  </si>
+  <si>
+    <t>#define TAG_KADMISCOPTIONS</t>
+  </si>
+  <si>
+    <t>\xF2</t>
+  </si>
+  <si>
+    <t>// &lt;uint8&gt;</t>
+  </si>
+  <si>
+    <t>#define TAG_ENCRYPTION</t>
+  </si>
+  <si>
+    <t>\xF3</t>
+  </si>
+  <si>
+    <t>#define TAG_USER_COUNT</t>
+  </si>
+  <si>
+    <t>\xF4</t>
+  </si>
+  <si>
+    <t>#define TAG_FILE_COUNT</t>
+  </si>
+  <si>
+    <t>\xF5</t>
+  </si>
+  <si>
+    <t>#define  FT_FILECOMMENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0xF6</t>
+  </si>
+  <si>
+    <t>#define TAG_FILECOMMENT</t>
+  </si>
+  <si>
+    <t>\xF6</t>
+  </si>
+  <si>
+    <t>#define  FT_FILERATING</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0xF7</t>
+  </si>
+  <si>
+    <t>#define TAG_FILERATING</t>
+  </si>
+  <si>
+    <t>\xF7</t>
+  </si>
+  <si>
+    <t>#define TAG_BUDDYHASH</t>
+  </si>
+  <si>
+    <t>\xF8</t>
+  </si>
+  <si>
+    <t>#define TAG_CLIENTLOWID</t>
+  </si>
+  <si>
+    <t>\xF9</t>
+  </si>
+  <si>
+    <t>#define TAG_SERVERPORT</t>
+  </si>
+  <si>
+    <t>\xFA</t>
+  </si>
+  <si>
+    <t>// &lt;uint16&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0x01</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>#define TAG_SERVERIP</t>
+  </si>
+  <si>
+    <t>\xFB</t>
+  </si>
+  <si>
+    <t>#define TAG_SOURCEUPORT</t>
+  </si>
+  <si>
+    <t>\xFC</t>
+  </si>
+  <si>
+    <t>#define TAG_SOURCEPORT</t>
+  </si>
+  <si>
+    <t>\xFD</t>
+  </si>
+  <si>
+    <t>#define TAG_SOURCEIP</t>
+  </si>
+  <si>
+    <t>\xFE</t>
+  </si>
+  <si>
+    <t>#define TAG_SOURCETYPE</t>
+  </si>
+  <si>
+    <t>\xFF</t>
   </si>
 </sst>
 </file>
@@ -696,7 +1322,7 @@
   <dimension ref="B2:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -866,7 +1492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
@@ -878,13 +1504,13 @@
   <sheetData>
     <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="2:4" x14ac:dyDescent="0.2">
@@ -892,32 +1518,32 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D3" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="2:4" x14ac:dyDescent="0.2">
@@ -925,32 +1551,32 @@
         <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="9" spans="2:4" x14ac:dyDescent="0.2">
@@ -958,32 +1584,32 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.2">
@@ -991,32 +1617,32 @@
         <v>6</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.2">
@@ -1024,21 +1650,21 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C16" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -1046,32 +1672,32 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D18" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
@@ -1079,54 +1705,54 @@
         <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D20" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C21" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D22" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C23" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D23" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
@@ -1134,10 +1760,10 @@
         <v>10</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D25" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
@@ -1145,10 +1771,10 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D26" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
@@ -1156,21 +1782,21 @@
         <v>18</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D27" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C28" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D28" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
@@ -1178,21 +1804,21 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D29" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C30" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
@@ -1200,10 +1826,10 @@
         <v>19</v>
       </c>
       <c r="C31" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="D31" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
@@ -1211,54 +1837,54 @@
         <v>13</v>
       </c>
       <c r="C32" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D32" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C33" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C34" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="D34" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C35" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D35" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D36" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
@@ -1266,21 +1892,21 @@
         <v>14</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D37" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C38" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -1288,21 +1914,21 @@
         <v>20</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D39" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C40" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D40" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
@@ -1310,32 +1936,32 @@
         <v>16</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D41" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C42" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C43" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D43" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.2">
@@ -1343,32 +1969,32 @@
         <v>17</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D44" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B45" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C45" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D45" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C46" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
@@ -1376,10 +2002,10 @@
         <v>21</v>
       </c>
       <c r="C47" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D47" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
@@ -1387,10 +2013,10 @@
         <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D48" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
@@ -1398,10 +2024,10 @@
         <v>27</v>
       </c>
       <c r="C49" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D49" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
@@ -1409,21 +2035,21 @@
         <v>22</v>
       </c>
       <c r="C50" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="D50" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C51" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D51" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
@@ -1431,10 +2057,10 @@
         <v>23</v>
       </c>
       <c r="C52" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D52" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -1442,10 +2068,10 @@
         <v>24</v>
       </c>
       <c r="C53" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D53" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
@@ -1453,21 +2079,21 @@
         <v>26</v>
       </c>
       <c r="C54" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D54" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C55" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D55" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
@@ -1475,10 +2101,10 @@
         <v>28</v>
       </c>
       <c r="C56" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D56" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.2">
@@ -1486,21 +2112,21 @@
         <v>29</v>
       </c>
       <c r="C57" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="D57" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C58" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D58" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
@@ -1508,10 +2134,1140 @@
         <v>30</v>
       </c>
       <c r="C59" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D59" t="s">
-        <v>110</v>
+        <v>111</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C2:I99"/>
+  <sheetViews>
+    <sheetView topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="E98" sqref="E98"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="28.125" customWidth="1"/>
+    <col min="4" max="4" width="18.5" customWidth="1"/>
+    <col min="5" max="5" width="21.875" customWidth="1"/>
+    <col min="6" max="6" width="15.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F2" t="s">
+        <v>308</v>
+      </c>
+      <c r="G2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F5" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>122</v>
+      </c>
+      <c r="F6" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F7" t="s">
+        <v>125</v>
+      </c>
+      <c r="G7" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>126</v>
+      </c>
+      <c r="F8" t="s">
+        <v>127</v>
+      </c>
+      <c r="G8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>128</v>
+      </c>
+      <c r="F9" t="s">
+        <v>129</v>
+      </c>
+      <c r="G9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>130</v>
+      </c>
+      <c r="F10" t="s">
+        <v>131</v>
+      </c>
+      <c r="G10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+      <c r="F11" t="s">
+        <v>133</v>
+      </c>
+      <c r="G11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" t="s">
+        <v>135</v>
+      </c>
+      <c r="E12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>138</v>
+      </c>
+      <c r="G14" t="s">
+        <v>139</v>
+      </c>
+      <c r="H14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" t="s">
+        <v>140</v>
+      </c>
+      <c r="G15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>142</v>
+      </c>
+      <c r="F16" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>144</v>
+      </c>
+      <c r="G17" t="s">
+        <v>145</v>
+      </c>
+      <c r="H17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>146</v>
+      </c>
+      <c r="F18" t="s">
+        <v>147</v>
+      </c>
+      <c r="G18" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="19" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>148</v>
+      </c>
+      <c r="G19" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="20" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" t="s">
+        <v>151</v>
+      </c>
+      <c r="H20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>154</v>
+      </c>
+      <c r="F22" t="s">
+        <v>155</v>
+      </c>
+      <c r="G22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C23" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" t="s">
+        <v>156</v>
+      </c>
+      <c r="G23" t="s">
+        <v>157</v>
+      </c>
+      <c r="H23" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" t="s">
+        <v>158</v>
+      </c>
+      <c r="H24" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" t="s">
+        <v>160</v>
+      </c>
+      <c r="H25" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" t="s">
+        <v>162</v>
+      </c>
+      <c r="G26" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>164</v>
+      </c>
+      <c r="G27" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C28" t="s">
+        <v>166</v>
+      </c>
+      <c r="F28" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" t="s">
+        <v>169</v>
+      </c>
+      <c r="H29" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="30" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C30" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" t="s">
+        <v>171</v>
+      </c>
+      <c r="F30" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="31" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C31" t="s">
+        <v>172</v>
+      </c>
+      <c r="E31" t="s">
+        <v>173</v>
+      </c>
+      <c r="F31" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C32" t="s">
+        <v>174</v>
+      </c>
+      <c r="F32" t="s">
+        <v>175</v>
+      </c>
+      <c r="G32" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
+        <v>177</v>
+      </c>
+      <c r="F33" t="s">
+        <v>178</v>
+      </c>
+      <c r="G33" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>179</v>
+      </c>
+      <c r="G34" t="s">
+        <v>180</v>
+      </c>
+      <c r="H34" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
+        <v>181</v>
+      </c>
+      <c r="G35" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>183</v>
+      </c>
+      <c r="G36" t="s">
+        <v>184</v>
+      </c>
+      <c r="H36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C37" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" t="s">
+        <v>186</v>
+      </c>
+      <c r="H37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>187</v>
+      </c>
+      <c r="F38" t="s">
+        <v>188</v>
+      </c>
+      <c r="G38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C39" t="s">
+        <v>189</v>
+      </c>
+      <c r="F39" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C40" t="s">
+        <v>191</v>
+      </c>
+      <c r="F40" t="s">
+        <v>192</v>
+      </c>
+      <c r="G40" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>193</v>
+      </c>
+      <c r="G41" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>195</v>
+      </c>
+      <c r="F42" t="s">
+        <v>196</v>
+      </c>
+      <c r="G42" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>198</v>
+      </c>
+      <c r="F43" t="s">
+        <v>199</v>
+      </c>
+      <c r="G43" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>31</v>
+      </c>
+      <c r="D44" t="s">
+        <v>201</v>
+      </c>
+      <c r="G44" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>31</v>
+      </c>
+      <c r="D45" t="s">
+        <v>203</v>
+      </c>
+      <c r="G45" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C46" t="s">
+        <v>205</v>
+      </c>
+      <c r="D46" t="s">
+        <v>206</v>
+      </c>
+      <c r="E46" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C47" t="s">
+        <v>207</v>
+      </c>
+      <c r="D47" t="s">
+        <v>208</v>
+      </c>
+      <c r="E47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C48" t="s">
+        <v>31</v>
+      </c>
+      <c r="D48" t="s">
+        <v>209</v>
+      </c>
+      <c r="H48" t="s">
+        <v>210</v>
+      </c>
+      <c r="I48" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C49" t="s">
+        <v>31</v>
+      </c>
+      <c r="D49" t="s">
+        <v>211</v>
+      </c>
+      <c r="F49" t="s">
+        <v>212</v>
+      </c>
+      <c r="G49" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C50" t="s">
+        <v>31</v>
+      </c>
+      <c r="D50" t="s">
+        <v>213</v>
+      </c>
+      <c r="F50" t="s">
+        <v>214</v>
+      </c>
+      <c r="G50" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="51" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C51" t="s">
+        <v>215</v>
+      </c>
+      <c r="F51" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C52" t="s">
+        <v>217</v>
+      </c>
+      <c r="D52" t="s">
+        <v>218</v>
+      </c>
+      <c r="E52" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C53" t="s">
+        <v>220</v>
+      </c>
+      <c r="F53" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="54" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C54" t="s">
+        <v>222</v>
+      </c>
+      <c r="F54" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="55" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C55" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" t="s">
+        <v>224</v>
+      </c>
+      <c r="E55" t="s">
+        <v>225</v>
+      </c>
+      <c r="F55" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C56" t="s">
+        <v>227</v>
+      </c>
+      <c r="D56" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="57" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C57" t="s">
+        <v>229</v>
+      </c>
+      <c r="D57" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="58" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C58" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="59" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C59" t="s">
+        <v>232</v>
+      </c>
+      <c r="F59" t="s">
+        <v>233</v>
+      </c>
+      <c r="G59" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="60" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C60" t="s">
+        <v>234</v>
+      </c>
+      <c r="F60" t="s">
+        <v>235</v>
+      </c>
+      <c r="G60" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="61" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C61" t="s">
+        <v>236</v>
+      </c>
+      <c r="F61" t="s">
+        <v>237</v>
+      </c>
+      <c r="G61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C62" t="s">
+        <v>238</v>
+      </c>
+      <c r="F62" t="s">
+        <v>239</v>
+      </c>
+      <c r="G62" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C63" t="s">
+        <v>31</v>
+      </c>
+      <c r="D63" t="s">
+        <v>240</v>
+      </c>
+      <c r="F63" t="s">
+        <v>241</v>
+      </c>
+      <c r="G63" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="64" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C64" t="s">
+        <v>243</v>
+      </c>
+      <c r="D64" t="s">
+        <v>244</v>
+      </c>
+      <c r="E64" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C65" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C66" t="s">
+        <v>247</v>
+      </c>
+      <c r="E66" t="s">
+        <v>248</v>
+      </c>
+      <c r="F66" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C67" t="s">
+        <v>249</v>
+      </c>
+      <c r="F67" t="s">
+        <v>250</v>
+      </c>
+      <c r="G67" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C68" t="s">
+        <v>251</v>
+      </c>
+      <c r="F68" t="s">
+        <v>252</v>
+      </c>
+      <c r="G68" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C69" t="s">
+        <v>253</v>
+      </c>
+      <c r="F69" t="s">
+        <v>254</v>
+      </c>
+      <c r="G69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C70" t="s">
+        <v>31</v>
+      </c>
+      <c r="D70" t="s">
+        <v>255</v>
+      </c>
+      <c r="F70" t="s">
+        <v>256</v>
+      </c>
+      <c r="G70" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C71" t="s">
+        <v>31</v>
+      </c>
+      <c r="D71" t="s">
+        <v>257</v>
+      </c>
+      <c r="G71" t="s">
+        <v>258</v>
+      </c>
+      <c r="H71" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C72" t="s">
+        <v>31</v>
+      </c>
+      <c r="D72" t="s">
+        <v>259</v>
+      </c>
+      <c r="F72" t="s">
+        <v>260</v>
+      </c>
+      <c r="G72" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C73" t="s">
+        <v>31</v>
+      </c>
+      <c r="D73" t="s">
+        <v>261</v>
+      </c>
+      <c r="F73" t="s">
+        <v>262</v>
+      </c>
+      <c r="G73" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C74" t="s">
+        <v>31</v>
+      </c>
+      <c r="D74" t="s">
+        <v>263</v>
+      </c>
+      <c r="G74" t="s">
+        <v>264</v>
+      </c>
+      <c r="H74" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="75" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C75" t="s">
+        <v>31</v>
+      </c>
+      <c r="D75" t="s">
+        <v>265</v>
+      </c>
+      <c r="G75" t="s">
+        <v>266</v>
+      </c>
+      <c r="H75" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C76" t="s">
+        <v>31</v>
+      </c>
+      <c r="D76" t="s">
+        <v>267</v>
+      </c>
+      <c r="G76" t="s">
+        <v>268</v>
+      </c>
+      <c r="H76" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C77" t="s">
+        <v>31</v>
+      </c>
+      <c r="D77" t="s">
+        <v>269</v>
+      </c>
+      <c r="G77" t="s">
+        <v>270</v>
+      </c>
+      <c r="H77" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="78" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C78" t="s">
+        <v>31</v>
+      </c>
+      <c r="D78" t="s">
+        <v>271</v>
+      </c>
+      <c r="F78" t="s">
+        <v>272</v>
+      </c>
+      <c r="G78" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C79" t="s">
+        <v>31</v>
+      </c>
+      <c r="D79" t="s">
+        <v>274</v>
+      </c>
+      <c r="F79" t="s">
+        <v>275</v>
+      </c>
+      <c r="G79" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="80" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C80" t="s">
+        <v>31</v>
+      </c>
+      <c r="D80" t="s">
+        <v>276</v>
+      </c>
+      <c r="F80" t="s">
+        <v>277</v>
+      </c>
+      <c r="G80" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="81" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C81" t="s">
+        <v>31</v>
+      </c>
+      <c r="D81" t="s">
+        <v>278</v>
+      </c>
+      <c r="F81" t="s">
+        <v>279</v>
+      </c>
+      <c r="G81" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="82" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C82" t="s">
+        <v>31</v>
+      </c>
+      <c r="D82" t="s">
+        <v>280</v>
+      </c>
+      <c r="G82" t="s">
+        <v>281</v>
+      </c>
+      <c r="H82" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="83" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C83" t="s">
+        <v>31</v>
+      </c>
+      <c r="D83" t="s">
+        <v>282</v>
+      </c>
+      <c r="G83" t="s">
+        <v>283</v>
+      </c>
+      <c r="H83" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="84" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C84" t="s">
+        <v>284</v>
+      </c>
+      <c r="E84" t="s">
+        <v>285</v>
+      </c>
+      <c r="F84" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="85" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>287</v>
+      </c>
+      <c r="F85" t="s">
+        <v>288</v>
+      </c>
+      <c r="G85" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="86" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>289</v>
+      </c>
+      <c r="F86" t="s">
+        <v>290</v>
+      </c>
+      <c r="G86" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="87" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>291</v>
+      </c>
+      <c r="F87" t="s">
+        <v>292</v>
+      </c>
+      <c r="G87" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="88" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>293</v>
+      </c>
+      <c r="F88" t="s">
+        <v>294</v>
+      </c>
+      <c r="G88" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="89" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>295</v>
+      </c>
+      <c r="F89" t="s">
+        <v>296</v>
+      </c>
+      <c r="G89" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="90" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>297</v>
+      </c>
+      <c r="F90" t="s">
+        <v>298</v>
+      </c>
+      <c r="G90" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="91" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>299</v>
+      </c>
+      <c r="F91" t="s">
+        <v>300</v>
+      </c>
+      <c r="G91" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="92" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>301</v>
+      </c>
+      <c r="F92" t="s">
+        <v>302</v>
+      </c>
+      <c r="G92" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="93" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>303</v>
+      </c>
+      <c r="F93" t="s">
+        <v>304</v>
+      </c>
+      <c r="G93" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>305</v>
+      </c>
+      <c r="F94" t="s">
+        <v>306</v>
+      </c>
+      <c r="G94" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="95" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C95" t="s">
+        <v>309</v>
+      </c>
+      <c r="F95" t="s">
+        <v>310</v>
+      </c>
+      <c r="G95" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="96" spans="3:8" x14ac:dyDescent="0.2">
+      <c r="C96" t="s">
+        <v>311</v>
+      </c>
+      <c r="F96" t="s">
+        <v>312</v>
+      </c>
+      <c r="G96" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="97" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C97" t="s">
+        <v>313</v>
+      </c>
+      <c r="F97" t="s">
+        <v>314</v>
+      </c>
+      <c r="G97" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="98" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C98" t="s">
+        <v>315</v>
+      </c>
+      <c r="F98" t="s">
+        <v>316</v>
+      </c>
+      <c r="G98" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="99" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="C99" t="s">
+        <v>317</v>
+      </c>
+      <c r="F99" t="s">
+        <v>318</v>
+      </c>
+      <c r="G99" t="s">
+        <v>286</v>
       </c>
     </row>
   </sheetData>

</xml_diff>